<commit_message>
acessibilidade e atualização cronograma
</commit_message>
<xml_diff>
--- a/proj/ConvidadosCasamento.xlsx
+++ b/proj/ConvidadosCasamento.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\alura-git\proj\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorio\alura-git\proj\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27430731-DEE5-4868-AF3A-A7B6C5769C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="283">
   <si>
     <t>Padrinhos</t>
   </si>
@@ -868,12 +869,18 @@
   </si>
   <si>
     <t>Samuel Lopes</t>
+  </si>
+  <si>
+    <t>Ir João</t>
+  </si>
+  <si>
+    <t>Irmã Telma</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -1314,11 +1321,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:S112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+      <selection activeCell="Q101" sqref="Q101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3885,6 +3892,9 @@
       <c r="L105" s="4">
         <v>294</v>
       </c>
+      <c r="M105" s="1" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="106" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H106" s="6"/>
@@ -3898,6 +3908,9 @@
       <c r="L106" s="4">
         <v>295</v>
       </c>
+      <c r="M106" s="1" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="107" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H107" s="6"/>
@@ -3910,6 +3923,9 @@
       <c r="K107" s="6"/>
       <c r="L107" s="4">
         <v>296</v>
+      </c>
+      <c r="M107" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="108" spans="8:13" x14ac:dyDescent="0.25">
@@ -3984,7 +4000,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
já prometido jogo de panelas e marcado quem recebeu o convite digital
</commit_message>
<xml_diff>
--- a/proj/ConvidadosCasamento.xlsx
+++ b/proj/ConvidadosCasamento.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorio\alura-git\proj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27430731-DEE5-4868-AF3A-A7B6C5769C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F298CF30-FDDA-44D9-8A49-BF8BF6143F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="282">
   <si>
     <t>Padrinhos</t>
   </si>
@@ -524,9 +524,6 @@
   </si>
   <si>
     <t>Maria</t>
-  </si>
-  <si>
-    <t>Irmão do Gustavo</t>
   </si>
   <si>
     <t>Julio</t>
@@ -939,7 +936,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -988,6 +985,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1003,7 +1006,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1028,6 +1031,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -1325,7 +1329,7 @@
   <dimension ref="A3:S112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q101" sqref="Q101"/>
+      <selection activeCell="R93" sqref="R93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1352,34 +1356,34 @@
   <sheetData>
     <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="9" t="s">
         <v>1</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="9" t="s">
         <v>62</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="L3" s="4"/>
       <c r="P3" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="R3" s="3" t="s">
         <v>190</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>191</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>149</v>
@@ -1387,13 +1391,13 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E4" s="6">
         <v>1</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>18</v>
@@ -1401,7 +1405,7 @@
       <c r="H4" s="6">
         <v>26</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <v>84</v>
       </c>
       <c r="J4" s="3" t="s">
@@ -1410,11 +1414,11 @@
       <c r="K4" s="6">
         <v>58</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="3">
         <v>193</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P4" s="2" t="s">
         <v>96</v>
@@ -1436,21 +1440,21 @@
         <v>5</v>
       </c>
       <c r="H5" s="6"/>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <v>85</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>64</v>
       </c>
       <c r="K5" s="6"/>
-      <c r="L5" s="4">
+      <c r="L5" s="3">
         <v>194</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -1460,21 +1464,21 @@
       <c r="E6" s="6">
         <v>2</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="2">
         <v>2</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H6" s="6"/>
-      <c r="I6" s="4">
+      <c r="I6" s="3">
         <v>86</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>65</v>
       </c>
       <c r="K6" s="6"/>
-      <c r="L6" s="4">
+      <c r="L6" s="3">
         <v>195</v>
       </c>
       <c r="M6" s="3" t="s">
@@ -1484,13 +1488,13 @@
         <v>146</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -1498,31 +1502,31 @@
         <v>1</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E7" s="6"/>
-      <c r="F7" s="4">
+      <c r="F7" s="2">
         <v>3</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H7" s="6"/>
-      <c r="I7" s="4">
+      <c r="I7" s="3">
         <v>87</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>66</v>
       </c>
       <c r="K7" s="6"/>
-      <c r="L7" s="4">
+      <c r="L7" s="3">
         <v>196</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="Q7" s="2" t="s">
         <v>95</v>
@@ -1542,7 +1546,7 @@
         <v>150</v>
       </c>
       <c r="E8" s="6"/>
-      <c r="F8" s="4">
+      <c r="F8" s="2">
         <v>4</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -1551,7 +1555,7 @@
       <c r="H8" s="6">
         <v>27</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="2">
         <v>88</v>
       </c>
       <c r="J8" s="2" t="s">
@@ -1560,17 +1564,17 @@
       <c r="K8" s="6">
         <v>59</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8" s="2">
         <v>197</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="S8" s="2" t="s">
         <v>102</v>
@@ -1581,33 +1585,33 @@
         <v>3</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E9" s="6">
         <v>3</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>5</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H9" s="6"/>
-      <c r="I9" s="4">
+      <c r="I9" s="2">
         <v>89</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>68</v>
       </c>
       <c r="K9" s="6"/>
-      <c r="L9" s="4">
+      <c r="L9" s="2">
         <v>198</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -1620,28 +1624,28 @@
       <c r="E10" s="6">
         <v>4</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>6</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>7</v>
       </c>
       <c r="H10" s="6"/>
-      <c r="I10" s="4">
+      <c r="I10" s="2">
         <v>90</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="16" t="s">
         <v>69</v>
       </c>
       <c r="K10" s="6"/>
-      <c r="L10" s="4">
+      <c r="L10" s="2">
         <v>199</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -1649,31 +1653,31 @@
         <v>5</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E11" s="6"/>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>7</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>8</v>
       </c>
       <c r="H11" s="6"/>
-      <c r="I11" s="4">
+      <c r="I11" s="2">
         <v>91</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>70</v>
       </c>
       <c r="K11" s="6"/>
-      <c r="L11" s="4">
+      <c r="L11" s="2">
         <v>200</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -1681,12 +1685,12 @@
         <v>6</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E12" s="6">
         <v>5</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="2">
         <v>8</v>
       </c>
       <c r="G12" s="2" t="s">
@@ -1695,21 +1699,21 @@
       <c r="H12" s="6">
         <v>28</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="2">
         <v>92</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K12" s="6"/>
-      <c r="L12" s="4">
+      <c r="L12" s="2">
         <v>201</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -1722,14 +1726,14 @@
       <c r="E13" s="6">
         <v>6</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="3">
         <v>9</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>10</v>
       </c>
       <c r="H13" s="6"/>
-      <c r="I13" s="4">
+      <c r="I13" s="2">
         <v>93</v>
       </c>
       <c r="J13" s="1" t="s">
@@ -1738,11 +1742,11 @@
       <c r="K13" s="6">
         <v>60</v>
       </c>
-      <c r="L13" s="4">
+      <c r="L13" s="3">
         <v>202</v>
       </c>
-      <c r="M13" s="3" t="s">
-        <v>176</v>
+      <c r="M13" s="16" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -1753,24 +1757,24 @@
         <v>151</v>
       </c>
       <c r="E14" s="6"/>
-      <c r="F14" s="4">
+      <c r="F14" s="3">
         <v>10</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>11</v>
       </c>
       <c r="H14" s="6"/>
-      <c r="I14" s="4">
+      <c r="I14" s="2">
         <v>94</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>74</v>
       </c>
       <c r="K14" s="6"/>
-      <c r="L14" s="4">
+      <c r="L14" s="3">
         <v>203</v>
       </c>
-      <c r="M14" s="3" t="s">
+      <c r="M14" s="16" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1779,10 +1783,10 @@
         <v>9</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E15" s="6"/>
-      <c r="F15" s="4">
+      <c r="F15" s="3">
         <v>11</v>
       </c>
       <c r="G15" s="3" t="s">
@@ -1791,17 +1795,17 @@
       <c r="H15" s="6">
         <v>29</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15" s="3">
         <v>95</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>75</v>
       </c>
       <c r="K15" s="6"/>
-      <c r="L15" s="4">
+      <c r="L15" s="3">
         <v>204</v>
       </c>
-      <c r="M15" s="3" t="s">
+      <c r="M15" s="16" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1810,10 +1814,10 @@
         <v>10</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E16" s="6"/>
-      <c r="F16" s="4">
+      <c r="F16" s="3">
         <v>12</v>
       </c>
       <c r="G16" s="3" t="s">
@@ -1822,16 +1826,16 @@
       <c r="H16" s="6">
         <v>30</v>
       </c>
-      <c r="I16" s="4">
+      <c r="I16" s="3">
         <v>96</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K16" s="6">
         <v>61</v>
       </c>
-      <c r="L16" s="4">
+      <c r="L16" s="2">
         <v>205</v>
       </c>
       <c r="M16" s="2" t="s">
@@ -1842,21 +1846,21 @@
       <c r="E17" s="6">
         <v>7</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="2">
         <v>13</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H17" s="6"/>
-      <c r="I17" s="4">
+      <c r="I17" s="3">
         <v>97</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>76</v>
       </c>
       <c r="K17" s="6"/>
-      <c r="L17" s="4">
+      <c r="L17" s="2">
         <v>206</v>
       </c>
       <c r="M17" s="2" t="s">
@@ -1865,21 +1869,21 @@
     </row>
     <row r="18" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E18" s="6"/>
-      <c r="F18" s="4">
+      <c r="F18" s="2">
         <v>14</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>78</v>
       </c>
       <c r="H18" s="6"/>
-      <c r="I18" s="4">
+      <c r="I18" s="3">
         <v>98</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>50</v>
       </c>
       <c r="K18" s="6"/>
-      <c r="L18" s="4">
+      <c r="L18" s="2">
         <v>207</v>
       </c>
       <c r="M18" s="2" t="s">
@@ -1890,7 +1894,7 @@
       <c r="E19" s="6">
         <v>8</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="3">
         <v>15</v>
       </c>
       <c r="G19" s="3" t="s">
@@ -1899,14 +1903,14 @@
       <c r="H19" s="6">
         <v>31</v>
       </c>
-      <c r="I19" s="4">
+      <c r="I19" s="2">
         <v>99</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>93</v>
       </c>
       <c r="K19" s="6"/>
-      <c r="L19" s="4">
+      <c r="L19" s="2">
         <v>208</v>
       </c>
       <c r="M19" s="2" t="s">
@@ -1915,21 +1919,21 @@
     </row>
     <row r="20" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E20" s="6"/>
-      <c r="F20" s="4">
+      <c r="F20" s="3">
         <v>16</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H20" s="6"/>
-      <c r="I20" s="4">
+      <c r="I20" s="2">
         <v>100</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>94</v>
       </c>
       <c r="K20" s="6"/>
-      <c r="L20" s="4">
+      <c r="L20" s="2">
         <v>209</v>
       </c>
       <c r="M20" s="2" t="s">
@@ -1940,21 +1944,21 @@
     </row>
     <row r="21" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E21" s="6"/>
-      <c r="F21" s="4">
+      <c r="F21" s="3">
         <v>17</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>79</v>
       </c>
       <c r="H21" s="6"/>
-      <c r="I21" s="4">
+      <c r="I21" s="2">
         <v>101</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>95</v>
       </c>
       <c r="K21" s="6"/>
-      <c r="L21" s="4">
+      <c r="L21" s="2">
         <v>210</v>
       </c>
       <c r="M21" s="2" t="s">
@@ -1964,7 +1968,7 @@
     </row>
     <row r="22" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E22" s="6"/>
-      <c r="F22" s="4">
+      <c r="F22" s="3">
         <v>18</v>
       </c>
       <c r="G22" s="3" t="s">
@@ -1973,14 +1977,14 @@
       <c r="H22" s="6">
         <v>32</v>
       </c>
-      <c r="I22" s="4">
+      <c r="I22" s="3">
         <v>102</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>96</v>
       </c>
       <c r="K22" s="6"/>
-      <c r="L22" s="4">
+      <c r="L22" s="2">
         <v>211</v>
       </c>
       <c r="M22" s="2" t="s">
@@ -1991,14 +1995,14 @@
       <c r="E23" s="6">
         <v>9</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="2">
         <v>19</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H23" s="6"/>
-      <c r="I23" s="4">
+      <c r="I23" s="3">
         <v>103</v>
       </c>
       <c r="J23" s="3" t="s">
@@ -2007,7 +2011,7 @@
       <c r="K23" s="6">
         <v>62</v>
       </c>
-      <c r="L23" s="4">
+      <c r="L23" s="3">
         <v>212</v>
       </c>
       <c r="M23" s="3" t="s">
@@ -2016,21 +2020,21 @@
     </row>
     <row r="24" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E24" s="6"/>
-      <c r="F24" s="4">
+      <c r="F24" s="2">
         <v>20</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>20</v>
       </c>
       <c r="H24" s="6"/>
-      <c r="I24" s="4">
+      <c r="I24" s="3">
         <v>104</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>98</v>
       </c>
       <c r="K24" s="6"/>
-      <c r="L24" s="4">
+      <c r="L24" s="3">
         <v>213</v>
       </c>
       <c r="M24" s="3" t="s">
@@ -2039,21 +2043,21 @@
     </row>
     <row r="25" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E25" s="6"/>
-      <c r="F25" s="4">
+      <c r="F25" s="2">
         <v>21</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H25" s="6"/>
-      <c r="I25" s="4">
+      <c r="I25" s="3">
         <v>105</v>
       </c>
       <c r="J25" s="3" t="s">
         <v>99</v>
       </c>
       <c r="K25" s="6"/>
-      <c r="L25" s="4">
+      <c r="L25" s="3">
         <v>214</v>
       </c>
       <c r="M25" s="3" t="s">
@@ -2064,21 +2068,21 @@
       <c r="E26" s="6">
         <v>10</v>
       </c>
-      <c r="F26" s="4">
+      <c r="F26" s="3">
         <v>22</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>22</v>
       </c>
       <c r="H26" s="6"/>
-      <c r="I26" s="4">
+      <c r="I26" s="3">
         <v>106</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>16</v>
       </c>
       <c r="K26" s="6"/>
-      <c r="L26" s="4">
+      <c r="L26" s="3">
         <v>215</v>
       </c>
       <c r="M26" s="3" t="s">
@@ -2087,14 +2091,14 @@
     </row>
     <row r="27" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E27" s="6"/>
-      <c r="F27" s="4">
+      <c r="F27" s="3">
         <v>23</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>20</v>
       </c>
       <c r="H27" s="6"/>
-      <c r="I27" s="4">
+      <c r="I27" s="3">
         <v>107</v>
       </c>
       <c r="J27" s="3" t="s">
@@ -2103,10 +2107,10 @@
       <c r="K27" s="6">
         <v>63</v>
       </c>
-      <c r="L27" s="4">
+      <c r="L27" s="2">
         <v>216</v>
       </c>
-      <c r="M27" s="2" t="s">
+      <c r="M27" s="16" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2114,71 +2118,71 @@
       <c r="E28" s="6">
         <v>11</v>
       </c>
-      <c r="F28" s="4">
+      <c r="F28" s="2">
         <v>24</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G28" s="16" t="s">
         <v>52</v>
       </c>
       <c r="H28" s="6">
         <v>34</v>
       </c>
-      <c r="I28" s="4">
+      <c r="I28" s="2">
         <v>108</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K28" s="6"/>
-      <c r="L28" s="4">
+      <c r="L28" s="2">
         <v>217</v>
       </c>
-      <c r="M28" s="2" t="s">
+      <c r="M28" s="16" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="29" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E29" s="6"/>
-      <c r="F29" s="4">
+      <c r="F29" s="2">
         <v>25</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G29" s="16" t="s">
         <v>81</v>
       </c>
       <c r="H29" s="6"/>
-      <c r="I29" s="4">
+      <c r="I29" s="2">
         <v>109</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K29" s="6"/>
-      <c r="L29" s="4">
+      <c r="L29" s="2">
         <v>218</v>
       </c>
-      <c r="M29" s="2" t="s">
+      <c r="M29" s="16" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="30" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E30" s="6"/>
-      <c r="F30" s="4">
+      <c r="F30" s="2">
         <v>26</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G30" s="16" t="s">
         <v>79</v>
       </c>
       <c r="H30" s="6"/>
-      <c r="I30" s="4">
+      <c r="I30" s="2">
         <v>110</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K30" s="6">
         <v>64</v>
       </c>
-      <c r="L30" s="4">
+      <c r="L30" s="3">
         <v>219</v>
       </c>
       <c r="M30" s="3" t="s">
@@ -2187,21 +2191,21 @@
     </row>
     <row r="31" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E31" s="6"/>
-      <c r="F31" s="4">
+      <c r="F31" s="2">
         <v>27</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="G31" s="16" t="s">
         <v>82</v>
       </c>
       <c r="H31" s="6"/>
-      <c r="I31" s="4">
+      <c r="I31" s="2">
         <v>111</v>
       </c>
       <c r="J31" s="2" t="s">
         <v>33</v>
       </c>
       <c r="K31" s="6"/>
-      <c r="L31" s="4">
+      <c r="L31" s="3">
         <v>220</v>
       </c>
       <c r="M31" s="3" t="s">
@@ -2210,21 +2214,21 @@
     </row>
     <row r="32" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E32" s="6"/>
-      <c r="F32" s="4">
+      <c r="F32" s="2">
         <v>28</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="G32" s="16" t="s">
         <v>41</v>
       </c>
       <c r="H32" s="6"/>
-      <c r="I32" s="4">
+      <c r="I32" s="2">
         <v>112</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>47</v>
       </c>
       <c r="K32" s="6"/>
-      <c r="L32" s="4">
+      <c r="L32" s="3">
         <v>221</v>
       </c>
       <c r="M32" s="3" t="s">
@@ -2235,7 +2239,7 @@
       <c r="E33" s="6">
         <v>12</v>
       </c>
-      <c r="F33" s="4">
+      <c r="F33" s="3">
         <v>29</v>
       </c>
       <c r="G33" s="3" t="s">
@@ -2244,14 +2248,14 @@
       <c r="H33" s="6">
         <v>35</v>
       </c>
-      <c r="I33" s="4">
+      <c r="I33" s="3">
         <v>113</v>
       </c>
       <c r="J33" s="3" t="s">
         <v>105</v>
       </c>
       <c r="K33" s="6"/>
-      <c r="L33" s="4">
+      <c r="L33" s="3">
         <v>222</v>
       </c>
       <c r="M33" s="3" t="s">
@@ -2260,21 +2264,21 @@
     </row>
     <row r="34" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E34" s="6"/>
-      <c r="F34" s="4">
+      <c r="F34" s="3">
         <v>30</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>24</v>
       </c>
       <c r="H34" s="6"/>
-      <c r="I34" s="4">
+      <c r="I34" s="3">
         <v>114</v>
       </c>
       <c r="J34" s="3" t="s">
         <v>106</v>
       </c>
       <c r="K34" s="6"/>
-      <c r="L34" s="4">
+      <c r="L34" s="3">
         <v>223</v>
       </c>
       <c r="M34" s="3" t="s">
@@ -2285,7 +2289,7 @@
       <c r="E35" s="6">
         <v>13</v>
       </c>
-      <c r="F35" s="4">
+      <c r="F35" s="2">
         <v>31</v>
       </c>
       <c r="G35" s="2" t="s">
@@ -2294,7 +2298,7 @@
       <c r="H35" s="6">
         <v>36</v>
       </c>
-      <c r="I35" s="4">
+      <c r="I35" s="2">
         <v>115</v>
       </c>
       <c r="J35" s="2" t="s">
@@ -2303,62 +2307,62 @@
       <c r="K35" s="6">
         <v>65</v>
       </c>
-      <c r="L35" s="4">
+      <c r="L35" s="2">
         <v>224</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="36" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E36" s="6"/>
-      <c r="F36" s="4">
+      <c r="F36" s="2">
         <v>32</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>26</v>
       </c>
       <c r="H36" s="6"/>
-      <c r="I36" s="4">
+      <c r="I36" s="2">
         <v>116</v>
       </c>
       <c r="J36" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K36" s="6"/>
-      <c r="L36" s="4">
+      <c r="L36" s="2">
         <v>225</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="37" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E37" s="6"/>
-      <c r="F37" s="4">
+      <c r="F37" s="2">
         <v>33</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>27</v>
       </c>
       <c r="H37" s="6"/>
-      <c r="I37" s="4">
+      <c r="I37" s="2">
         <v>117</v>
       </c>
       <c r="J37" s="2" t="s">
         <v>74</v>
       </c>
       <c r="K37" s="6"/>
-      <c r="L37" s="4">
+      <c r="L37" s="2">
         <v>226</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="38" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E38" s="6"/>
-      <c r="F38" s="4">
+      <c r="F38" s="2">
         <v>34</v>
       </c>
       <c r="G38" s="2" t="s">
@@ -2367,16 +2371,16 @@
       <c r="H38" s="6">
         <v>37</v>
       </c>
-      <c r="I38" s="4">
+      <c r="I38" s="3">
         <v>118</v>
       </c>
-      <c r="J38" s="3" t="s">
+      <c r="J38" s="16" t="s">
         <v>108</v>
       </c>
       <c r="K38" s="6">
         <v>66</v>
       </c>
-      <c r="L38" s="4">
+      <c r="L38" s="3">
         <v>227</v>
       </c>
       <c r="M38" s="3" t="s">
@@ -2387,30 +2391,30 @@
       <c r="E39" s="6">
         <v>14</v>
       </c>
-      <c r="F39" s="4">
+      <c r="F39" s="3">
         <v>35</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>29</v>
       </c>
       <c r="H39" s="6"/>
-      <c r="I39" s="4">
+      <c r="I39" s="3">
         <v>119</v>
       </c>
-      <c r="J39" s="3" t="s">
+      <c r="J39" s="16" t="s">
         <v>109</v>
       </c>
       <c r="K39" s="6"/>
-      <c r="L39" s="4">
+      <c r="L39" s="3">
         <v>228</v>
       </c>
       <c r="M39" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="40" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E40" s="6"/>
-      <c r="F40" s="4">
+      <c r="F40" s="3">
         <v>36</v>
       </c>
       <c r="G40" s="3" t="s">
@@ -2419,53 +2423,53 @@
       <c r="H40" s="6">
         <v>38</v>
       </c>
-      <c r="I40" s="4">
+      <c r="I40" s="2">
         <v>120</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K40" s="6"/>
-      <c r="L40" s="4">
+      <c r="L40" s="3">
         <v>229</v>
       </c>
       <c r="M40" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="41" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E41" s="6"/>
-      <c r="F41" s="4">
+      <c r="F41" s="3">
         <v>37</v>
       </c>
       <c r="G41" s="3" t="s">
         <v>83</v>
       </c>
       <c r="H41" s="6"/>
-      <c r="I41" s="4">
+      <c r="I41" s="2">
         <v>121</v>
       </c>
       <c r="J41" s="2" t="s">
         <v>55</v>
       </c>
       <c r="K41" s="6"/>
-      <c r="L41" s="4">
+      <c r="L41" s="3">
         <v>230</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="42" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E42" s="6"/>
-      <c r="F42" s="4">
+      <c r="F42" s="3">
         <v>38</v>
       </c>
       <c r="G42" s="3" t="s">
         <v>30</v>
       </c>
       <c r="H42" s="6"/>
-      <c r="I42" s="4">
+      <c r="I42" s="2">
         <v>122</v>
       </c>
       <c r="J42" s="2" t="s">
@@ -2474,18 +2478,18 @@
       <c r="K42" s="6">
         <v>67</v>
       </c>
-      <c r="L42" s="4">
+      <c r="L42" s="2">
         <v>231</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="43" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E43" s="6">
         <v>15</v>
       </c>
-      <c r="F43" s="4">
+      <c r="F43" s="2">
         <v>39</v>
       </c>
       <c r="G43" s="2" t="s">
@@ -2494,53 +2498,53 @@
       <c r="H43" s="6">
         <v>39</v>
       </c>
-      <c r="I43" s="4">
+      <c r="I43" s="3">
         <v>123</v>
       </c>
       <c r="J43" s="3" t="s">
         <v>45</v>
       </c>
       <c r="K43" s="6"/>
-      <c r="L43" s="4">
+      <c r="L43" s="2">
         <v>232</v>
       </c>
       <c r="M43" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="44" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E44" s="6"/>
-      <c r="F44" s="4">
+      <c r="F44" s="2">
         <v>40</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>32</v>
       </c>
       <c r="H44" s="6"/>
-      <c r="I44" s="4">
+      <c r="I44" s="3">
         <v>124</v>
       </c>
       <c r="J44" s="3" t="s">
         <v>110</v>
       </c>
       <c r="K44" s="6"/>
-      <c r="L44" s="4">
+      <c r="L44" s="2">
         <v>233</v>
       </c>
       <c r="M44" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="45" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E45" s="6"/>
-      <c r="F45" s="4">
+      <c r="F45" s="2">
         <v>41</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>33</v>
       </c>
       <c r="H45" s="6"/>
-      <c r="I45" s="4">
+      <c r="I45" s="3">
         <v>125</v>
       </c>
       <c r="J45" s="3" t="s">
@@ -2549,16 +2553,16 @@
       <c r="K45" s="6">
         <v>68</v>
       </c>
-      <c r="L45" s="4">
+      <c r="L45" s="3">
         <v>234</v>
       </c>
       <c r="M45" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="46" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E46" s="6"/>
-      <c r="F46" s="4">
+      <c r="F46" s="2">
         <v>42</v>
       </c>
       <c r="G46" s="2" t="s">
@@ -2567,48 +2571,48 @@
       <c r="H46" s="6">
         <v>40</v>
       </c>
-      <c r="I46" s="4">
+      <c r="I46" s="2">
         <v>126</v>
       </c>
       <c r="J46" s="2" t="s">
         <v>158</v>
       </c>
       <c r="K46" s="6"/>
-      <c r="L46" s="4">
+      <c r="L46" s="3">
         <v>235</v>
       </c>
       <c r="M46" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="47" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E47" s="6">
         <v>16</v>
       </c>
-      <c r="F47" s="4">
+      <c r="F47" s="3">
         <v>43</v>
       </c>
       <c r="G47" s="3" t="s">
         <v>34</v>
       </c>
       <c r="H47" s="6"/>
-      <c r="I47" s="4">
+      <c r="I47" s="2">
         <v>127</v>
       </c>
       <c r="J47" s="2" t="s">
         <v>55</v>
       </c>
       <c r="K47" s="6"/>
-      <c r="L47" s="4">
+      <c r="L47" s="3">
         <v>236</v>
       </c>
       <c r="M47" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="48" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E48" s="6"/>
-      <c r="F48" s="4">
+      <c r="F48" s="3">
         <v>44</v>
       </c>
       <c r="G48" s="3" t="s">
@@ -2617,39 +2621,39 @@
       <c r="H48" s="6">
         <v>41</v>
       </c>
-      <c r="I48" s="4">
+      <c r="I48" s="3">
         <v>128</v>
       </c>
       <c r="J48" s="3" t="s">
         <v>128</v>
       </c>
       <c r="K48" s="6"/>
-      <c r="L48" s="4">
+      <c r="L48" s="3">
         <v>237</v>
       </c>
       <c r="M48" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="49" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E49" s="6"/>
-      <c r="F49" s="4">
+      <c r="F49" s="3">
         <v>45</v>
       </c>
       <c r="G49" s="3" t="s">
         <v>36</v>
       </c>
       <c r="H49" s="6"/>
-      <c r="I49" s="4">
+      <c r="I49" s="3">
         <v>129</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K49" s="6">
         <v>69</v>
       </c>
-      <c r="L49" s="4">
+      <c r="L49" s="2">
         <v>238</v>
       </c>
       <c r="M49" s="2" t="s">
@@ -2658,32 +2662,32 @@
     </row>
     <row r="50" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E50" s="6"/>
-      <c r="F50" s="4">
+      <c r="F50" s="3">
         <v>46</v>
       </c>
       <c r="G50" s="3" t="s">
         <v>37</v>
       </c>
       <c r="H50" s="6"/>
-      <c r="I50" s="4">
+      <c r="I50" s="3">
         <v>130</v>
       </c>
       <c r="J50" s="3" t="s">
         <v>129</v>
       </c>
       <c r="K50" s="6"/>
-      <c r="L50" s="4">
+      <c r="L50" s="2">
         <v>239</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="51" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E51" s="6">
         <v>17</v>
       </c>
-      <c r="F51" s="4">
+      <c r="F51" s="2">
         <v>47</v>
       </c>
       <c r="G51" s="2" t="s">
@@ -2692,53 +2696,53 @@
       <c r="H51" s="6">
         <v>42</v>
       </c>
-      <c r="I51" s="4">
+      <c r="I51" s="2">
         <v>131</v>
       </c>
       <c r="J51" s="2" t="s">
         <v>111</v>
       </c>
       <c r="K51" s="6"/>
-      <c r="L51" s="4">
+      <c r="L51" s="2">
         <v>240</v>
       </c>
       <c r="M51" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="52" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E52" s="6"/>
-      <c r="F52" s="4">
+      <c r="F52" s="2">
         <v>48</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>39</v>
       </c>
       <c r="H52" s="6"/>
-      <c r="I52" s="4">
+      <c r="I52" s="2">
         <v>132</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>112</v>
       </c>
       <c r="K52" s="6"/>
-      <c r="L52" s="4">
+      <c r="L52" s="2">
         <v>241</v>
       </c>
       <c r="M52" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="53" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E53" s="6"/>
-      <c r="F53" s="4">
+      <c r="F53" s="2">
         <v>49</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H53" s="6"/>
-      <c r="I53" s="4">
+      <c r="I53" s="2">
         <v>133</v>
       </c>
       <c r="J53" s="2" t="s">
@@ -2747,62 +2751,62 @@
       <c r="K53" s="6">
         <v>70</v>
       </c>
-      <c r="L53" s="4">
+      <c r="L53" s="3">
         <v>242</v>
       </c>
       <c r="M53" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="54" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E54" s="6"/>
-      <c r="F54" s="4">
+      <c r="F54" s="2">
         <v>50</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>85</v>
       </c>
       <c r="H54" s="6"/>
-      <c r="I54" s="4">
+      <c r="I54" s="2">
         <v>134</v>
       </c>
       <c r="J54" s="2" t="s">
         <v>65</v>
       </c>
       <c r="K54" s="6"/>
-      <c r="L54" s="4">
+      <c r="L54" s="3">
         <v>243</v>
       </c>
       <c r="M54" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="55" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E55" s="6"/>
-      <c r="F55" s="4">
+      <c r="F55" s="2">
         <v>51</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>33</v>
       </c>
       <c r="H55" s="6"/>
-      <c r="I55" s="4">
+      <c r="I55" s="2">
         <v>135</v>
       </c>
       <c r="J55" s="2" t="s">
         <v>15</v>
       </c>
       <c r="K55" s="6"/>
-      <c r="L55" s="4">
+      <c r="L55" s="3">
         <v>244</v>
       </c>
       <c r="M55" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="56" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E56" s="6"/>
-      <c r="F56" s="4">
+      <c r="F56" s="2">
         <v>52</v>
       </c>
       <c r="G56" s="2" t="s">
@@ -2811,32 +2815,32 @@
       <c r="H56" s="6">
         <v>43</v>
       </c>
-      <c r="I56" s="4">
+      <c r="I56" s="3">
         <v>136</v>
       </c>
       <c r="J56" s="3" t="s">
         <v>113</v>
       </c>
       <c r="K56" s="6"/>
-      <c r="L56" s="4">
+      <c r="L56" s="3">
         <v>245</v>
       </c>
       <c r="M56" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="57" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E57" s="6">
         <v>18</v>
       </c>
-      <c r="F57" s="4">
+      <c r="F57" s="3">
         <v>53</v>
       </c>
-      <c r="G57" s="3" t="s">
+      <c r="G57" s="16" t="s">
         <v>51</v>
       </c>
       <c r="H57" s="6"/>
-      <c r="I57" s="4">
+      <c r="I57" s="3">
         <v>137</v>
       </c>
       <c r="J57" s="3" t="s">
@@ -2845,73 +2849,73 @@
       <c r="K57" s="6">
         <v>71</v>
       </c>
-      <c r="L57" s="4">
+      <c r="L57" s="2">
         <v>246</v>
       </c>
       <c r="M57" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="58" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E58" s="6"/>
-      <c r="F58" s="4">
+      <c r="F58" s="3">
         <v>54</v>
       </c>
-      <c r="G58" s="3" t="s">
+      <c r="G58" s="16" t="s">
         <v>43</v>
       </c>
       <c r="H58" s="6"/>
-      <c r="I58" s="4">
+      <c r="I58" s="3">
         <v>138</v>
       </c>
       <c r="J58" s="3" t="s">
         <v>115</v>
       </c>
       <c r="K58" s="6"/>
-      <c r="L58" s="4">
+      <c r="L58" s="2">
         <v>247</v>
       </c>
       <c r="M58" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="59" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E59" s="6">
         <v>19</v>
       </c>
-      <c r="F59" s="4">
+      <c r="F59" s="2">
         <v>55</v>
       </c>
-      <c r="G59" s="2" t="s">
+      <c r="G59" s="16" t="s">
         <v>44</v>
       </c>
       <c r="H59" s="6"/>
-      <c r="I59" s="4">
+      <c r="I59" s="3">
         <v>139</v>
       </c>
       <c r="J59" s="3" t="s">
         <v>116</v>
       </c>
       <c r="K59" s="6"/>
-      <c r="L59" s="4">
+      <c r="L59" s="2">
         <v>248</v>
       </c>
       <c r="M59" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="60" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E60" s="6"/>
-      <c r="F60" s="4">
+      <c r="F60" s="2">
         <v>56</v>
       </c>
-      <c r="G60" s="2" t="s">
+      <c r="G60" s="16" t="s">
         <v>45</v>
       </c>
       <c r="H60" s="6">
         <v>44</v>
       </c>
-      <c r="I60" s="4">
+      <c r="I60" s="2">
         <v>140</v>
       </c>
       <c r="J60" s="2" t="s">
@@ -2920,105 +2924,105 @@
       <c r="K60" s="6">
         <v>72</v>
       </c>
-      <c r="L60" s="4">
+      <c r="L60" s="3">
         <v>249</v>
       </c>
       <c r="M60" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="61" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E61" s="6">
         <v>20</v>
       </c>
-      <c r="F61" s="4">
+      <c r="F61" s="3">
         <v>57</v>
       </c>
-      <c r="G61" s="3" t="s">
+      <c r="G61" s="16" t="s">
         <v>46</v>
       </c>
       <c r="H61" s="6"/>
-      <c r="I61" s="4">
+      <c r="I61" s="2">
         <v>141</v>
       </c>
       <c r="J61" s="2" t="s">
         <v>118</v>
       </c>
       <c r="K61" s="6"/>
-      <c r="L61" s="4">
+      <c r="L61" s="3">
         <v>250</v>
       </c>
       <c r="M61" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="62" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E62" s="6"/>
-      <c r="F62" s="4">
+      <c r="F62" s="3">
         <v>58</v>
       </c>
-      <c r="G62" s="3" t="s">
+      <c r="G62" s="16" t="s">
         <v>47</v>
       </c>
       <c r="H62" s="6"/>
-      <c r="I62" s="4">
+      <c r="I62" s="2">
         <v>142</v>
       </c>
       <c r="J62" s="2" t="s">
         <v>114</v>
       </c>
       <c r="K62" s="6"/>
-      <c r="L62" s="4">
+      <c r="L62" s="3">
         <v>251</v>
       </c>
       <c r="M62" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="63" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E63" s="6">
         <v>21</v>
       </c>
-      <c r="F63" s="4">
+      <c r="F63" s="2">
         <v>59</v>
       </c>
-      <c r="G63" s="2" t="s">
+      <c r="G63" s="16" t="s">
         <v>48</v>
       </c>
       <c r="H63" s="6"/>
-      <c r="I63" s="4">
+      <c r="I63" s="2">
         <v>143</v>
       </c>
       <c r="J63" s="2" t="s">
         <v>119</v>
       </c>
       <c r="K63" s="6"/>
-      <c r="L63" s="4">
+      <c r="L63" s="3">
         <v>252</v>
       </c>
       <c r="M63" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="64" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E64" s="6"/>
-      <c r="F64" s="4">
+      <c r="F64" s="2">
         <v>60</v>
       </c>
-      <c r="G64" s="2" t="s">
+      <c r="G64" s="16" t="s">
         <v>49</v>
       </c>
       <c r="H64" s="6"/>
-      <c r="I64" s="4">
+      <c r="I64" s="2">
         <v>144</v>
       </c>
       <c r="J64" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K64" s="6">
         <v>73</v>
       </c>
-      <c r="L64" s="4">
+      <c r="L64" s="2">
         <v>253</v>
       </c>
       <c r="M64" s="2" t="s">
@@ -3027,16 +3031,16 @@
     </row>
     <row r="65" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E65" s="6"/>
-      <c r="F65" s="4">
+      <c r="F65" s="2">
         <v>61</v>
       </c>
-      <c r="G65" s="2" t="s">
+      <c r="G65" s="16" t="s">
         <v>50</v>
       </c>
       <c r="H65" s="6">
         <v>45</v>
       </c>
-      <c r="I65" s="4">
+      <c r="I65" s="3">
         <v>145</v>
       </c>
       <c r="J65" s="3" t="s">
@@ -3045,85 +3049,85 @@
       <c r="K65" s="6">
         <v>74</v>
       </c>
-      <c r="L65" s="4">
+      <c r="L65" s="3">
         <v>254</v>
       </c>
       <c r="M65" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="66" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E66" s="6"/>
-      <c r="F66" s="4">
+      <c r="F66" s="2">
         <v>62</v>
       </c>
-      <c r="G66" s="2" t="s">
+      <c r="G66" s="16" t="s">
         <v>86</v>
       </c>
       <c r="H66" s="6"/>
-      <c r="I66" s="4">
+      <c r="I66" s="3">
         <v>146</v>
       </c>
       <c r="J66" s="3" t="s">
         <v>121</v>
       </c>
       <c r="K66" s="6"/>
-      <c r="L66" s="4">
+      <c r="L66" s="3">
         <v>255</v>
       </c>
       <c r="M66" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="67" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E67" s="6"/>
-      <c r="F67" s="4">
+      <c r="F67" s="2">
         <v>63</v>
       </c>
-      <c r="G67" s="2" t="s">
+      <c r="G67" s="16" t="s">
         <v>54</v>
       </c>
       <c r="H67" s="6"/>
-      <c r="I67" s="4">
+      <c r="I67" s="3">
         <v>147</v>
       </c>
       <c r="J67" s="3" t="s">
         <v>83</v>
       </c>
       <c r="K67" s="6"/>
-      <c r="L67" s="4">
+      <c r="L67" s="3">
         <v>256</v>
       </c>
       <c r="M67" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="68" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E68" s="6"/>
-      <c r="F68" s="4">
+      <c r="F68" s="2">
         <v>64</v>
       </c>
-      <c r="G68" s="2" t="s">
+      <c r="G68" s="16" t="s">
         <v>55</v>
       </c>
       <c r="H68" s="6"/>
-      <c r="I68" s="4">
+      <c r="I68" s="3">
         <v>148</v>
       </c>
       <c r="J68" s="3" t="s">
         <v>122</v>
       </c>
       <c r="K68" s="6"/>
-      <c r="L68" s="4">
+      <c r="L68" s="3">
         <v>257</v>
       </c>
       <c r="M68" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="69" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E69" s="6"/>
-      <c r="F69" s="4">
+      <c r="F69" s="2">
         <v>65</v>
       </c>
       <c r="G69" s="2" t="s">
@@ -3132,30 +3136,30 @@
       <c r="H69" s="6">
         <v>46</v>
       </c>
-      <c r="I69" s="4">
+      <c r="I69" s="2">
         <v>149</v>
       </c>
       <c r="J69" s="2" t="s">
         <v>123</v>
       </c>
       <c r="K69" s="6"/>
-      <c r="L69" s="4">
+      <c r="L69" s="3">
         <v>258</v>
       </c>
       <c r="M69" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="70" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E70" s="6"/>
-      <c r="F70" s="4">
+      <c r="F70" s="2">
         <v>66</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>88</v>
       </c>
       <c r="H70" s="6"/>
-      <c r="I70" s="4">
+      <c r="I70" s="2">
         <v>150</v>
       </c>
       <c r="J70" s="2" t="s">
@@ -3164,123 +3168,123 @@
       <c r="K70" s="6">
         <v>75</v>
       </c>
-      <c r="L70" s="4">
+      <c r="L70" s="2">
         <v>259</v>
       </c>
       <c r="M70" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="71" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E71" s="6">
         <v>22</v>
       </c>
-      <c r="F71" s="4">
+      <c r="F71" s="3">
         <v>67</v>
       </c>
       <c r="G71" s="3" t="s">
         <v>56</v>
       </c>
       <c r="H71" s="6"/>
-      <c r="I71" s="4">
+      <c r="I71" s="2">
         <v>151</v>
       </c>
       <c r="J71" s="2" t="s">
         <v>124</v>
       </c>
       <c r="K71" s="6"/>
-      <c r="L71" s="4">
+      <c r="L71" s="2">
         <v>260</v>
       </c>
       <c r="M71" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="72" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E72" s="6">
         <v>23</v>
       </c>
-      <c r="F72" s="4">
+      <c r="F72" s="2">
         <v>68</v>
       </c>
-      <c r="G72" s="2" t="s">
+      <c r="G72" s="16" t="s">
         <v>57</v>
       </c>
       <c r="H72" s="6">
         <v>47</v>
       </c>
-      <c r="I72" s="4">
+      <c r="I72" s="3">
         <v>152</v>
       </c>
       <c r="J72" s="3" t="s">
         <v>125</v>
       </c>
       <c r="K72" s="6"/>
-      <c r="L72" s="4">
+      <c r="L72" s="2">
         <v>261</v>
       </c>
       <c r="M72" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="73" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E73" s="6"/>
-      <c r="F73" s="4">
+      <c r="F73" s="2">
         <v>69</v>
       </c>
-      <c r="G73" s="2" t="s">
+      <c r="G73" s="16" t="s">
         <v>59</v>
       </c>
       <c r="H73" s="6"/>
-      <c r="I73" s="4">
+      <c r="I73" s="3">
         <v>153</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K73" s="6"/>
-      <c r="L73" s="4">
+      <c r="L73" s="2">
         <v>262</v>
       </c>
       <c r="M73" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="74" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E74" s="6"/>
-      <c r="F74" s="4">
+      <c r="F74" s="2">
         <v>70</v>
       </c>
-      <c r="G74" s="2" t="s">
+      <c r="G74" s="16" t="s">
         <v>58</v>
       </c>
       <c r="H74" s="6"/>
-      <c r="I74" s="4">
+      <c r="I74" s="3">
         <v>154</v>
       </c>
       <c r="J74" s="3" t="s">
         <v>127</v>
       </c>
       <c r="K74" s="6"/>
-      <c r="L74" s="4">
+      <c r="L74" s="2">
         <v>263</v>
       </c>
       <c r="M74" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="75" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E75" s="6"/>
-      <c r="F75" s="4">
+      <c r="F75" s="2">
         <v>71</v>
       </c>
-      <c r="G75" s="2" t="s">
+      <c r="G75" s="16" t="s">
         <v>60</v>
       </c>
       <c r="H75" s="6">
         <v>48</v>
       </c>
-      <c r="I75" s="4">
+      <c r="I75" s="2">
         <v>155</v>
       </c>
       <c r="J75" s="2" t="s">
@@ -3289,7 +3293,7 @@
       <c r="K75" s="6">
         <v>76</v>
       </c>
-      <c r="L75" s="4">
+      <c r="L75" s="3">
         <v>264</v>
       </c>
       <c r="M75" s="3" t="s">
@@ -3298,62 +3302,62 @@
     </row>
     <row r="76" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E76" s="6"/>
-      <c r="F76" s="4">
+      <c r="F76" s="2">
         <v>72</v>
       </c>
-      <c r="G76" s="2" t="s">
+      <c r="G76" s="16" t="s">
         <v>61</v>
       </c>
       <c r="H76" s="6"/>
-      <c r="I76" s="4">
+      <c r="I76" s="2">
         <v>156</v>
       </c>
       <c r="J76" s="2" t="s">
         <v>131</v>
       </c>
       <c r="K76" s="6"/>
-      <c r="L76" s="4">
+      <c r="L76" s="3">
         <v>265</v>
       </c>
       <c r="M76" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="77" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E77" s="6">
         <v>24</v>
       </c>
-      <c r="F77" s="4">
+      <c r="F77" s="3">
         <v>73</v>
       </c>
-      <c r="G77" s="3" t="s">
+      <c r="G77" s="16" t="s">
         <v>89</v>
       </c>
       <c r="H77" s="6"/>
-      <c r="I77" s="4">
+      <c r="I77" s="2">
         <v>157</v>
       </c>
       <c r="J77" s="2" t="s">
         <v>132</v>
       </c>
       <c r="K77" s="6"/>
-      <c r="L77" s="4">
+      <c r="L77" s="3">
         <v>266</v>
       </c>
       <c r="M77" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="78" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E78" s="6"/>
-      <c r="F78" s="4">
+      <c r="F78" s="3">
         <v>74</v>
       </c>
-      <c r="G78" s="3" t="s">
+      <c r="G78" s="16" t="s">
         <v>90</v>
       </c>
       <c r="H78" s="6"/>
-      <c r="I78" s="4">
+      <c r="I78" s="2">
         <v>158</v>
       </c>
       <c r="J78" s="2" t="s">
@@ -3362,219 +3366,219 @@
       <c r="K78" s="6">
         <v>77</v>
       </c>
-      <c r="L78" s="4">
+      <c r="L78" s="2">
         <v>267</v>
       </c>
       <c r="M78" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="79" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E79" s="6"/>
-      <c r="F79" s="4">
+      <c r="F79" s="3">
         <v>75</v>
       </c>
-      <c r="G79" s="3" t="s">
+      <c r="G79" s="16" t="s">
         <v>79</v>
       </c>
       <c r="H79" s="6"/>
-      <c r="I79" s="4">
+      <c r="I79" s="2">
         <v>159</v>
       </c>
       <c r="J79" s="2" t="s">
         <v>134</v>
       </c>
       <c r="K79" s="6"/>
-      <c r="L79" s="4">
+      <c r="L79" s="2">
         <v>268</v>
       </c>
       <c r="M79" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="80" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E80" s="6"/>
-      <c r="F80" s="4">
+      <c r="F80" s="3">
         <v>76</v>
       </c>
-      <c r="G80" s="3" t="s">
+      <c r="G80" s="16" t="s">
         <v>30</v>
       </c>
       <c r="H80" s="6">
         <v>49</v>
       </c>
-      <c r="I80" s="4">
+      <c r="I80" s="3">
         <v>160</v>
       </c>
-      <c r="J80" s="3" t="s">
+      <c r="J80" s="16" t="s">
         <v>138</v>
       </c>
       <c r="K80" s="6"/>
-      <c r="L80" s="4">
+      <c r="L80" s="2">
         <v>269</v>
       </c>
       <c r="M80" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="81" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E81" s="6"/>
-      <c r="F81" s="4">
+      <c r="F81" s="3">
         <v>77</v>
       </c>
-      <c r="G81" s="3" t="s">
+      <c r="G81" s="16" t="s">
         <v>30</v>
       </c>
       <c r="H81" s="6"/>
-      <c r="I81" s="4">
+      <c r="I81" s="3">
         <v>161</v>
       </c>
-      <c r="J81" s="3" t="s">
+      <c r="J81" s="16" t="s">
         <v>139</v>
       </c>
       <c r="K81" s="6">
         <v>78</v>
       </c>
-      <c r="L81" s="4">
+      <c r="L81" s="3">
         <v>270</v>
       </c>
       <c r="M81" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="82" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E82" s="6">
         <v>25</v>
       </c>
-      <c r="F82" s="4">
+      <c r="F82" s="2">
         <v>78</v>
       </c>
-      <c r="G82" s="2" t="s">
+      <c r="G82" s="16" t="s">
         <v>91</v>
       </c>
       <c r="H82" s="6">
         <v>50</v>
       </c>
-      <c r="I82" s="4">
+      <c r="I82" s="2">
         <v>162</v>
       </c>
-      <c r="J82" s="2" t="s">
+      <c r="J82" s="16" t="s">
         <v>140</v>
       </c>
       <c r="K82" s="6"/>
-      <c r="L82" s="4">
+      <c r="L82" s="3">
         <v>271</v>
       </c>
       <c r="M82" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="83" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E83" s="6"/>
-      <c r="F83" s="4">
+      <c r="F83" s="2">
         <v>79</v>
       </c>
-      <c r="G83" s="2" t="s">
+      <c r="G83" s="16" t="s">
         <v>92</v>
       </c>
       <c r="H83" s="6"/>
-      <c r="I83" s="4">
+      <c r="I83" s="2">
         <v>163</v>
       </c>
-      <c r="J83" s="2" t="s">
+      <c r="J83" s="16" t="s">
         <v>55</v>
       </c>
       <c r="K83" s="6"/>
-      <c r="L83" s="4">
+      <c r="L83" s="3">
         <v>272</v>
       </c>
       <c r="M83" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="84" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E84" s="6"/>
-      <c r="F84" s="4">
+      <c r="F84" s="2">
         <v>80</v>
       </c>
-      <c r="G84" s="2" t="s">
+      <c r="G84" s="16" t="s">
         <v>50</v>
       </c>
       <c r="H84" s="6">
         <v>51</v>
       </c>
-      <c r="I84" s="4">
+      <c r="I84" s="3">
         <v>164</v>
       </c>
       <c r="J84" s="3" t="s">
         <v>141</v>
       </c>
       <c r="K84" s="6"/>
-      <c r="L84" s="4">
+      <c r="L84" s="3">
         <v>273</v>
       </c>
       <c r="M84" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="85" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E85" s="6"/>
-      <c r="F85" s="4">
+      <c r="F85" s="2">
         <v>81</v>
       </c>
-      <c r="G85" s="2" t="s">
+      <c r="G85" s="16" t="s">
         <v>86</v>
       </c>
       <c r="H85" s="6"/>
-      <c r="I85" s="4">
+      <c r="I85" s="3">
         <v>165</v>
       </c>
       <c r="J85" s="3" t="s">
         <v>142</v>
       </c>
       <c r="K85" s="6"/>
-      <c r="L85" s="4">
+      <c r="L85" s="3">
         <v>274</v>
       </c>
       <c r="M85" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="86" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E86" s="6"/>
-      <c r="F86" s="4">
+      <c r="F86" s="2">
         <v>82</v>
       </c>
-      <c r="G86" s="2" t="s">
-        <v>180</v>
+      <c r="G86" s="16" t="s">
+        <v>179</v>
       </c>
       <c r="H86" s="6">
         <v>52</v>
       </c>
-      <c r="I86" s="4">
+      <c r="I86" s="2">
         <v>166</v>
       </c>
       <c r="J86" s="2" t="s">
         <v>143</v>
       </c>
       <c r="K86" s="6"/>
-      <c r="L86" s="4">
+      <c r="L86" s="3">
         <v>275</v>
       </c>
       <c r="M86" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="87" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E87" s="6"/>
-      <c r="F87" s="4">
+      <c r="F87" s="2">
         <v>83</v>
       </c>
-      <c r="G87" s="2" t="s">
-        <v>181</v>
+      <c r="G87" s="16" t="s">
+        <v>180</v>
       </c>
       <c r="H87" s="6"/>
-      <c r="I87" s="4">
+      <c r="I87" s="2">
         <v>167</v>
       </c>
       <c r="J87" s="2" t="s">
@@ -3583,66 +3587,66 @@
       <c r="K87" s="6">
         <v>79</v>
       </c>
-      <c r="L87" s="4">
+      <c r="L87" s="2">
         <v>276</v>
       </c>
       <c r="M87" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="88" spans="5:13" x14ac:dyDescent="0.25">
       <c r="H88" s="6">
         <v>53</v>
       </c>
-      <c r="I88" s="4">
+      <c r="I88" s="3">
         <v>168</v>
       </c>
       <c r="J88" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K88" s="6"/>
-      <c r="L88" s="4">
+      <c r="L88" s="2">
         <v>277</v>
       </c>
       <c r="M88" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="89" spans="5:13" x14ac:dyDescent="0.25">
       <c r="H89" s="6"/>
-      <c r="I89" s="4">
+      <c r="I89" s="3">
         <v>169</v>
       </c>
       <c r="J89" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K89" s="6"/>
-      <c r="L89" s="4">
+      <c r="L89" s="2">
         <v>278</v>
       </c>
       <c r="M89" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="90" spans="5:13" x14ac:dyDescent="0.25">
       <c r="H90" s="6"/>
-      <c r="I90" s="4">
+      <c r="I90" s="3">
         <v>170</v>
       </c>
       <c r="J90" s="3" t="s">
         <v>145</v>
       </c>
       <c r="K90" s="6"/>
-      <c r="L90" s="4">
+      <c r="L90" s="2">
         <v>279</v>
       </c>
       <c r="M90" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="91" spans="5:13" x14ac:dyDescent="0.25">
       <c r="H91" s="6"/>
-      <c r="I91" s="4">
+      <c r="I91" s="3">
         <v>171</v>
       </c>
       <c r="J91" s="3" t="s">
@@ -3651,68 +3655,68 @@
       <c r="K91" s="6">
         <v>80</v>
       </c>
-      <c r="L91" s="4">
+      <c r="L91" s="3">
         <v>280</v>
       </c>
       <c r="M91" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="92" spans="5:13" x14ac:dyDescent="0.25">
       <c r="H92" s="6">
         <v>54</v>
       </c>
-      <c r="I92" s="4">
+      <c r="I92" s="2">
         <v>172</v>
       </c>
       <c r="J92" s="2" t="s">
         <v>147</v>
       </c>
       <c r="K92" s="6"/>
-      <c r="L92" s="4">
+      <c r="L92" s="3">
         <v>281</v>
       </c>
       <c r="M92" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="93" spans="5:13" x14ac:dyDescent="0.25">
       <c r="H93" s="6"/>
-      <c r="I93" s="4">
+      <c r="I93" s="2">
         <v>173</v>
       </c>
       <c r="J93" s="2" t="s">
         <v>55</v>
       </c>
       <c r="K93" s="6"/>
-      <c r="L93" s="4">
+      <c r="L93" s="3">
         <v>282</v>
       </c>
       <c r="M93" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="94" spans="5:13" x14ac:dyDescent="0.25">
       <c r="H94" s="6"/>
-      <c r="I94" s="4">
+      <c r="I94" s="2">
         <v>174</v>
       </c>
       <c r="J94" s="2" t="s">
         <v>148</v>
       </c>
       <c r="K94" s="6"/>
-      <c r="L94" s="4">
+      <c r="L94" s="3">
         <v>283</v>
       </c>
       <c r="M94" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="95" spans="5:13" x14ac:dyDescent="0.25">
       <c r="H95" s="6">
         <v>55</v>
       </c>
-      <c r="I95" s="4">
+      <c r="I95" s="3">
         <v>175</v>
       </c>
       <c r="J95" s="3" t="s">
@@ -3721,207 +3725,207 @@
       <c r="K95" s="6">
         <v>81</v>
       </c>
-      <c r="L95" s="4">
+      <c r="L95" s="2">
         <v>284</v>
       </c>
       <c r="M95" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="96" spans="5:13" x14ac:dyDescent="0.25">
       <c r="H96" s="6"/>
-      <c r="I96" s="4">
+      <c r="I96" s="3">
         <v>176</v>
       </c>
       <c r="J96" s="3" t="s">
         <v>82</v>
       </c>
       <c r="K96" s="6"/>
-      <c r="L96" s="4">
+      <c r="L96" s="2">
         <v>285</v>
       </c>
       <c r="M96" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="97" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H97" s="6"/>
-      <c r="I97" s="4">
+      <c r="I97" s="3">
         <v>177</v>
       </c>
-      <c r="J97" s="3" t="s">
+      <c r="J97" s="16" t="s">
         <v>61</v>
       </c>
       <c r="K97" s="6"/>
-      <c r="L97" s="4">
+      <c r="L97" s="2">
         <v>286</v>
       </c>
       <c r="M97" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="98" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H98" s="6"/>
-      <c r="I98" s="4">
+      <c r="I98" s="3">
         <v>178</v>
       </c>
-      <c r="J98" s="3" t="s">
+      <c r="J98" s="16" t="s">
         <v>55</v>
       </c>
       <c r="K98" s="6">
         <v>82</v>
       </c>
-      <c r="L98" s="4">
+      <c r="L98" s="3">
         <v>287</v>
       </c>
       <c r="M98" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="99" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H99" s="6"/>
-      <c r="I99" s="4">
+      <c r="I99" s="3">
         <v>179</v>
       </c>
       <c r="J99" s="3" t="s">
         <v>7</v>
       </c>
       <c r="K99" s="6"/>
-      <c r="L99" s="4">
+      <c r="L99" s="3">
         <v>288</v>
       </c>
       <c r="M99" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="100" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H100" s="6"/>
-      <c r="I100" s="4">
+      <c r="I100" s="3">
         <v>180</v>
       </c>
       <c r="J100" s="3" t="s">
         <v>53</v>
       </c>
       <c r="K100" s="6"/>
-      <c r="L100" s="4">
+      <c r="L100" s="3">
         <v>289</v>
       </c>
       <c r="M100" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="101" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H101" s="6">
         <v>56</v>
       </c>
-      <c r="I101" s="4">
+      <c r="I101" s="2">
         <v>181</v>
       </c>
-      <c r="J101" s="2" t="s">
+      <c r="J101" s="16" t="s">
         <v>155</v>
       </c>
       <c r="K101" s="6">
         <v>83</v>
       </c>
-      <c r="L101" s="4">
+      <c r="L101" s="2">
         <v>290</v>
       </c>
       <c r="M101" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="102" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H102" s="6"/>
-      <c r="I102" s="4">
+      <c r="I102" s="2">
         <v>182</v>
       </c>
-      <c r="J102" s="2" t="s">
+      <c r="J102" s="16" t="s">
         <v>55</v>
       </c>
       <c r="K102" s="6"/>
-      <c r="L102" s="4">
+      <c r="L102" s="2">
         <v>291</v>
       </c>
       <c r="M102" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="103" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H103" s="6"/>
-      <c r="I103" s="4">
+      <c r="I103" s="2">
         <v>183</v>
       </c>
       <c r="J103" s="2" t="s">
         <v>156</v>
       </c>
       <c r="K103" s="6"/>
-      <c r="L103" s="4">
+      <c r="L103" s="2">
         <v>292</v>
       </c>
       <c r="M103" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="104" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H104" s="6"/>
-      <c r="I104" s="4">
+      <c r="I104" s="2">
         <v>184</v>
       </c>
       <c r="J104" s="2" t="s">
         <v>157</v>
       </c>
       <c r="K104" s="6"/>
-      <c r="L104" s="4">
+      <c r="L104" s="2">
         <v>293</v>
       </c>
       <c r="M104" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="105" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H105" s="6">
         <v>57</v>
       </c>
-      <c r="I105" s="4">
+      <c r="I105" s="3">
         <v>185</v>
       </c>
-      <c r="J105" s="3" t="s">
+      <c r="J105" s="16" t="s">
         <v>164</v>
       </c>
       <c r="K105" s="6"/>
-      <c r="L105" s="4">
+      <c r="L105" s="3">
         <v>294</v>
       </c>
       <c r="M105" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="106" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H106" s="6"/>
-      <c r="I106" s="4">
+      <c r="I106" s="3">
         <v>186</v>
       </c>
-      <c r="J106" s="3" t="s">
+      <c r="J106" s="16" t="s">
         <v>126</v>
       </c>
       <c r="K106" s="6"/>
-      <c r="L106" s="4">
+      <c r="L106" s="3">
         <v>295</v>
       </c>
       <c r="M106" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="107" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H107" s="6"/>
-      <c r="I107" s="4">
+      <c r="I107" s="3">
         <v>187</v>
       </c>
-      <c r="J107" s="3" t="s">
+      <c r="J107" s="16" t="s">
         <v>162</v>
       </c>
       <c r="K107" s="6"/>
-      <c r="L107" s="4">
+      <c r="L107" s="3">
         <v>296</v>
       </c>
       <c r="M107" s="1" t="s">
@@ -3930,66 +3934,66 @@
     </row>
     <row r="108" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H108" s="6"/>
-      <c r="I108" s="4">
+      <c r="I108" s="3">
         <v>188</v>
       </c>
-      <c r="J108" s="3" t="s">
-        <v>65</v>
+      <c r="J108" s="16" t="s">
+        <v>165</v>
       </c>
       <c r="K108" s="6"/>
-      <c r="L108" s="4">
+      <c r="L108" s="2">
         <v>297</v>
       </c>
     </row>
     <row r="109" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H109" s="6"/>
-      <c r="I109" s="4">
+      <c r="I109" s="3">
         <v>189</v>
       </c>
-      <c r="J109" s="3" t="s">
-        <v>163</v>
+      <c r="J109" s="16" t="s">
+        <v>65</v>
       </c>
       <c r="K109" s="6"/>
-      <c r="L109" s="4">
+      <c r="L109" s="2">
         <v>298</v>
       </c>
     </row>
     <row r="110" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H110" s="6"/>
-      <c r="I110" s="4">
+      <c r="I110" s="3">
         <v>190</v>
       </c>
-      <c r="J110" s="3" t="s">
-        <v>165</v>
+      <c r="J110" s="16" t="s">
+        <v>163</v>
       </c>
       <c r="K110" s="6"/>
-      <c r="L110" s="4">
+      <c r="L110" s="2">
         <v>299</v>
       </c>
     </row>
     <row r="111" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H111" s="6"/>
-      <c r="I111" s="4">
+      <c r="I111" s="3">
         <v>191</v>
       </c>
-      <c r="J111" s="3" t="s">
-        <v>166</v>
+      <c r="J111" s="16" t="s">
+        <v>32</v>
       </c>
       <c r="K111" s="6"/>
-      <c r="L111" s="4">
+      <c r="L111" s="2">
         <v>300</v>
       </c>
     </row>
     <row r="112" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H112" s="6"/>
-      <c r="I112" s="4">
+      <c r="I112" s="3">
         <v>192</v>
       </c>
-      <c r="J112" s="3" t="s">
+      <c r="J112" s="16" t="s">
         <v>55</v>
       </c>
       <c r="K112" s="6"/>
-      <c r="L112" s="4">
+      <c r="L112" s="2">
         <v>301</v>
       </c>
     </row>
@@ -4015,7 +4019,7 @@
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C3" s="12">
         <v>30</v>
@@ -4026,7 +4030,7 @@
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C4" s="12">
         <v>50</v>
@@ -4037,7 +4041,7 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C5" s="12">
         <v>35</v>

</xml_diff>